<commit_message>
semi fix - excel matriz
</commit_message>
<xml_diff>
--- a/matriz_copia/Matriz Clashs_copia.xlsx
+++ b/matriz_copia/Matriz Clashs_copia.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="120">
   <si>
     <t>MATRIZ DE INTERFERÊNCIAS</t>
   </si>
@@ -396,22 +396,13 @@
   </si>
   <si>
     <t>Engastado</t>
-  </si>
-  <si>
-    <t>Drenagem Linear</t>
-  </si>
-  <si>
-    <t>Drenagem Enterrado</t>
-  </si>
-  <si>
-    <t>Drenagem Pontual</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -427,8 +418,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -453,8 +451,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -597,11 +619,54 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="2" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="medium">
+        <color theme="2" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -659,6 +724,24 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -994,19 +1077,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="24.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="14" width="5.25" customWidth="1"/>
+    <col min="3" max="12" width="5.25" customWidth="1"/>
+    <col min="13" max="13" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:14">
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1014,37 +1098,31 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="138">
+    <row r="2" spans="1:14" ht="138">
       <c r="B2" s="15" t="s">
         <v>11</v>
       </c>
@@ -1052,40 +1130,34 @@
         <v>12</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>120</v>
+        <v>13</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>121</v>
+        <v>14</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>122</v>
+        <v>15</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="24.75" customHeight="1">
+    <row r="3" spans="1:14" ht="24.75" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -1094,63 +1166,57 @@
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
+      <c r="E3" s="6"/>
       <c r="F3" s="7"/>
-      <c r="G3" s="6"/>
+      <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="8"/>
-    </row>
-    <row r="4" spans="1:16" ht="24.75" customHeight="1">
+      <c r="K3" s="6"/>
+      <c r="L3" s="8"/>
+    </row>
+    <row r="4" spans="1:14" ht="24.75" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>120</v>
+        <v>13</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="9"/>
-    </row>
-    <row r="5" spans="1:16" ht="24.75" customHeight="1">
+      <c r="L4" s="9"/>
+    </row>
+    <row r="5" spans="1:14" ht="24.75" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>121</v>
+        <v>14</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
+      <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="9"/>
-    </row>
-    <row r="6" spans="1:16" ht="24.75" customHeight="1">
+      <c r="K5" s="6"/>
+      <c r="L5" s="8"/>
+    </row>
+    <row r="6" spans="1:14" ht="24.75" customHeight="1">
       <c r="A6" s="5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>122</v>
+        <v>15</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -1161,16 +1227,14 @@
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="9"/>
-    </row>
-    <row r="7" spans="1:16" ht="24.75" customHeight="1">
+      <c r="L6" s="9"/>
+    </row>
+    <row r="7" spans="1:14" ht="24.75" customHeight="1">
       <c r="A7" s="5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -1179,18 +1243,16 @@
       <c r="G7" s="6"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
+      <c r="J7" s="6"/>
       <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="8"/>
-    </row>
-    <row r="8" spans="1:16" ht="24.75" customHeight="1">
+      <c r="L7" s="9"/>
+    </row>
+    <row r="8" spans="1:14" ht="24.75" customHeight="1">
       <c r="A8" s="5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -1201,16 +1263,14 @@
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="9"/>
-    </row>
-    <row r="9" spans="1:16" ht="24.75" customHeight="1">
+      <c r="L8" s="9"/>
+    </row>
+    <row r="9" spans="1:14" ht="24.75" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
@@ -1221,16 +1281,14 @@
       <c r="I9" s="6"/>
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="9"/>
-    </row>
-    <row r="10" spans="1:16" ht="24.75" customHeight="1">
+      <c r="L9" s="8"/>
+    </row>
+    <row r="10" spans="1:14" ht="24.75" customHeight="1">
       <c r="A10" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
@@ -1241,16 +1299,14 @@
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
       <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="9"/>
-    </row>
-    <row r="11" spans="1:16" ht="24.75" customHeight="1">
+      <c r="L10" s="9"/>
+    </row>
+    <row r="11" spans="1:14" ht="24.75" customHeight="1">
       <c r="A11" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
@@ -1261,83 +1317,39 @@
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="8"/>
-    </row>
-    <row r="12" spans="1:16" ht="24.75" customHeight="1">
-      <c r="A12" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="9"/>
-    </row>
-    <row r="13" spans="1:16" ht="24.75" customHeight="1">
-      <c r="A13" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="9"/>
-    </row>
-    <row r="14" spans="1:16" ht="24.75" customHeight="1" thickBot="1">
-      <c r="A14" s="10" t="s">
+      <c r="L11" s="9"/>
+    </row>
+    <row r="12" spans="1:14" ht="24.75" customHeight="1" thickBot="1">
+      <c r="A12" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B12" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
-      <c r="N14" s="12"/>
-    </row>
-    <row r="15" spans="1:16">
-      <c r="O15" s="16" t="s">
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="12"/>
+    </row>
+    <row r="13" spans="1:14" ht="14.25" customHeight="1">
+      <c r="M13" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="P15" s="17"/>
-    </row>
-    <row r="16" spans="1:16">
-      <c r="O16" s="18"/>
-      <c r="P16" s="19"/>
+      <c r="N13" s="17"/>
+    </row>
+    <row r="14" spans="1:14" ht="14.25" customHeight="1">
+      <c r="M14" s="18"/>
+      <c r="N14" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="O15:P16"/>
+    <mergeCell ref="M13:N14"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -1345,1057 +1357,1774 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D128"/>
+  <dimension ref="A1:E128"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="24.95" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="23.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.75" customWidth="1"/>
-    <col min="3" max="3" width="34.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.625" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.75" style="20" customWidth="1"/>
+    <col min="3" max="3" width="34.625" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.25" style="20" customWidth="1"/>
+    <col min="5" max="5" width="1.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" ht="24.95" customHeight="1" thickBot="1">
+      <c r="A1" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="25" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="D1" s="24" t="str">
+        <f>CONCATENATE(A1,E1,B1)</f>
+        <v>Disciplina Categoria</v>
+      </c>
+      <c r="E1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A2" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="21" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+      <c r="C2" s="21"/>
+      <c r="D2" s="21" t="str">
+        <f t="shared" ref="D2:D65" si="0">CONCATENATE(A2,E2,B2)</f>
+        <v>Topografia Pontual</v>
+      </c>
+      <c r="E2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A3" s="20" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
+      <c r="D3" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Topografia </v>
+      </c>
+      <c r="E3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A4" s="20" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
+      <c r="D4" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Topografia </v>
+      </c>
+      <c r="E4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A5" s="20" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
+      <c r="D5" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Topografia </v>
+      </c>
+      <c r="E5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A6" s="20" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
+      <c r="D6" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Topografia </v>
+      </c>
+      <c r="E6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A7" s="20" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
+      <c r="D7" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Topografia </v>
+      </c>
+      <c r="E7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A8" s="20" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="D8" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">Topografia </v>
+      </c>
+      <c r="E8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A9" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="20" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="D9" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Drenagem Linear</v>
+      </c>
+      <c r="E9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A10" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="20" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="D10" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Drenagem Linear</v>
+      </c>
+      <c r="E10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A11" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="20" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="D11" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Drenagem Linear</v>
+      </c>
+      <c r="E11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A12" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="20" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="D12" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Drenagem Linear</v>
+      </c>
+      <c r="E12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A13" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="20" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="D13" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Drenagem Linear</v>
+      </c>
+      <c r="E13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A14" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="20" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="D14" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Drenagem Linear</v>
+      </c>
+      <c r="E14" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A15" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="20" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="D15" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Drenagem Linear</v>
+      </c>
+      <c r="E15" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A16" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="20" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="D16" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Drenagem Linear</v>
+      </c>
+      <c r="E16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A17" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="20" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="D17" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Drenagem Linear</v>
+      </c>
+      <c r="E17" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A18" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="20" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="D18" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Drenagem Linear</v>
+      </c>
+      <c r="E18" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A19" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="20" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="D19" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Drenagem Linear</v>
+      </c>
+      <c r="E19" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A20" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="20" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="D20" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Drenagem Linear</v>
+      </c>
+      <c r="E20" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A21" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="20" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="D21" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Drenagem Enterrado</v>
+      </c>
+      <c r="E21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A22" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="20" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="D22" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Drenagem Enterrado</v>
+      </c>
+      <c r="E22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A23" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="20" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" t="s">
+      <c r="D23" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Drenagem Enterrado</v>
+      </c>
+      <c r="E23" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A24" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="20" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B25" t="s">
+      <c r="D24" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Drenagem Enterrado</v>
+      </c>
+      <c r="E24" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A25" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="20" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" t="s">
+      <c r="D25" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Drenagem Enterrado</v>
+      </c>
+      <c r="E25" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A26" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="20" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" t="s">
-        <v>13</v>
-      </c>
-      <c r="B27" t="s">
+      <c r="D26" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Drenagem Enterrado</v>
+      </c>
+      <c r="E26" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A27" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="20" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" t="s">
+      <c r="D27" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Drenagem Enterrado</v>
+      </c>
+      <c r="E27" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A28" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="20" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29" t="s">
+      <c r="D28" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Drenagem Enterrado</v>
+      </c>
+      <c r="E28" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A29" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="20" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" t="s">
-        <v>13</v>
-      </c>
-      <c r="B30" t="s">
+      <c r="D29" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Drenagem Enterrado</v>
+      </c>
+      <c r="E29" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A30" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="20" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" t="s">
-        <v>13</v>
-      </c>
-      <c r="B31" t="s">
+      <c r="D30" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Drenagem Enterrado</v>
+      </c>
+      <c r="E30" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A31" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="20" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" t="s">
-        <v>13</v>
-      </c>
-      <c r="B32" t="s">
+      <c r="D31" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Drenagem Enterrado</v>
+      </c>
+      <c r="E31" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A32" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" s="20" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" t="s">
-        <v>13</v>
-      </c>
-      <c r="B33" t="s">
+      <c r="D32" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Drenagem Enterrado</v>
+      </c>
+      <c r="E32" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A33" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="20" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" t="s">
-        <v>13</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="D33" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Drenagem Pontual</v>
+      </c>
+      <c r="E33" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A34" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="20" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
-        <v>13</v>
-      </c>
-      <c r="B35" t="s">
+      <c r="D34" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Drenagem Pontual</v>
+      </c>
+      <c r="E34" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A35" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="20" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" t="s">
-        <v>13</v>
-      </c>
-      <c r="B36" t="s">
+      <c r="D35" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Drenagem Pontual</v>
+      </c>
+      <c r="E35" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A36" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="20" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" t="s">
-        <v>13</v>
-      </c>
-      <c r="B37" t="s">
+      <c r="D36" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Drenagem Pontual</v>
+      </c>
+      <c r="E36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A37" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B37" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="20" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" t="s">
-        <v>13</v>
-      </c>
-      <c r="B38" t="s">
+      <c r="D37" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Drenagem Pontual</v>
+      </c>
+      <c r="E37" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A38" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="20" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" t="s">
-        <v>13</v>
-      </c>
-      <c r="B39" t="s">
+      <c r="D38" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Drenagem Pontual</v>
+      </c>
+      <c r="E38" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A39" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B39" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="20" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" t="s">
-        <v>13</v>
-      </c>
-      <c r="B40" t="s">
+      <c r="D39" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Drenagem Pontual</v>
+      </c>
+      <c r="E39" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A40" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B40" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="20" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" t="s">
-        <v>13</v>
-      </c>
-      <c r="B41" t="s">
+      <c r="D40" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Drenagem Pontual</v>
+      </c>
+      <c r="E40" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A41" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="20" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" t="s">
-        <v>13</v>
-      </c>
-      <c r="B42" t="s">
+      <c r="D41" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Drenagem Pontual</v>
+      </c>
+      <c r="E41" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A42" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B42" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="20" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" t="s">
-        <v>13</v>
-      </c>
-      <c r="B43" t="s">
+      <c r="D42" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Drenagem Pontual</v>
+      </c>
+      <c r="E42" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A43" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B43" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="20" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" t="s">
-        <v>13</v>
-      </c>
-      <c r="B44" t="s">
+      <c r="D43" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Drenagem Pontual</v>
+      </c>
+      <c r="E43" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A44" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B44" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="20" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" t="s">
-        <v>13</v>
-      </c>
-      <c r="B45" t="s">
+      <c r="D44" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Drenagem Pontual</v>
+      </c>
+      <c r="E44" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A45" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B45" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="20" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" t="s">
-        <v>13</v>
-      </c>
-      <c r="B46" t="s">
+      <c r="D45" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Drenagem Pontual</v>
+      </c>
+      <c r="E45" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A46" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B46" s="20" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" t="s">
-        <v>13</v>
-      </c>
-      <c r="B47" t="s">
+      <c r="D46" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Drenagem Pontual</v>
+      </c>
+      <c r="E46" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A47" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B47" s="20" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" t="s">
-        <v>13</v>
-      </c>
-      <c r="B48" t="s">
+      <c r="D47" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Drenagem Pontual</v>
+      </c>
+      <c r="E47" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A48" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B48" s="20" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" t="s">
+      <c r="D48" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Drenagem Pontual</v>
+      </c>
+      <c r="E48" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A49" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="20" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" t="s">
+      <c r="D49" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Interferências Enterrada</v>
+      </c>
+      <c r="E49" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A50" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="20" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" t="s">
+      <c r="D50" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Interferências Enterrada</v>
+      </c>
+      <c r="E50" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A51" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="20" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" t="s">
+      <c r="D51" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Interferências Enterrada</v>
+      </c>
+      <c r="E51" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A52" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="20" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" t="s">
+      <c r="D52" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Interferências Enterrada</v>
+      </c>
+      <c r="E52" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A53" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="20" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" t="s">
+      <c r="D53" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Interferências Enterrada</v>
+      </c>
+      <c r="E53" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A54" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="20" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" t="s">
+      <c r="D54" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Interferências Enterrada</v>
+      </c>
+      <c r="E54" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A55" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="20" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56" t="s">
+      <c r="D55" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Interferências Enterrada</v>
+      </c>
+      <c r="E55" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A56" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="20" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" t="s">
+      <c r="D56" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Interferências Enterrada</v>
+      </c>
+      <c r="E56" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A57" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="20" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" t="s">
+      <c r="D57" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Interferências Aerea</v>
+      </c>
+      <c r="E57" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A58" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="20" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59" t="s">
+      <c r="D58" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Interferências Aerea</v>
+      </c>
+      <c r="E58" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A59" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="20" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" t="s">
+      <c r="D59" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Interferências Aerea</v>
+      </c>
+      <c r="E59" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A60" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="20" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" t="s">
+      <c r="D60" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Interferências Pontual</v>
+      </c>
+      <c r="E60" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A61" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="20" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="A62" t="s">
+      <c r="D61" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Interferências Pontual</v>
+      </c>
+      <c r="E61" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A62" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="20" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="A63" t="s">
+      <c r="D62" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Interferências Pontual</v>
+      </c>
+      <c r="E62" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A63" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="20" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="A64" t="s">
+      <c r="D63" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Interferências Pontual</v>
+      </c>
+      <c r="E63" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A64" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="20" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65" t="s">
+      <c r="D64" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Interferências Pontual</v>
+      </c>
+      <c r="E64" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A65" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="20" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66" t="s">
+      <c r="D65" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Interferências Pontual</v>
+      </c>
+      <c r="E65" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A66" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="20" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="A67" t="s">
+      <c r="D66" s="20" t="str">
+        <f t="shared" ref="D66:D99" si="1">CONCATENATE(A66,E66,B66)</f>
+        <v>Interferências Pontual</v>
+      </c>
+      <c r="E66" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A67" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" s="20" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="A68" t="s">
+      <c r="D67" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>Sinalização Vertical Pontual</v>
+      </c>
+      <c r="E67" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A68" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" s="20" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" t="s">
+      <c r="D68" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>Sinalização Vertical Pontual</v>
+      </c>
+      <c r="E68" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A69" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" s="20" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="70" spans="1:3">
-      <c r="A70" t="s">
+      <c r="D69" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>Sinalização Vertical Pontual</v>
+      </c>
+      <c r="E69" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A70" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C70" s="20" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="71" spans="1:3">
-      <c r="A71" t="s">
+      <c r="D70" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>Dispositivo de Segurança Linear</v>
+      </c>
+      <c r="E70" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A71" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71" s="20" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="A72" t="s">
+      <c r="D71" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>Dispositivo de Segurança Linear</v>
+      </c>
+      <c r="E71" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A72" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C72" s="20" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="A73" t="s">
+      <c r="D72" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>Dispositivo de Segurança Linear</v>
+      </c>
+      <c r="E72" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A73" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C73" s="20" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="A74" t="s">
+      <c r="D73" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>Dispositivo de Segurança Linear</v>
+      </c>
+      <c r="E73" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A74" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" s="20" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="A75" t="s">
+      <c r="D74" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>Dispositivo de Segurança Linear</v>
+      </c>
+      <c r="E74" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A75" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75" s="20" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="76" spans="1:3">
-      <c r="A76" t="s">
+      <c r="D75" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>Dispositivo de Segurança Linear</v>
+      </c>
+      <c r="E75" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A76" s="20" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="77" spans="1:3">
-      <c r="A77" t="s">
+      <c r="D76" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">OAEs </v>
+      </c>
+      <c r="E76" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A77" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="20" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="78" spans="1:3">
-      <c r="A78" t="s">
+      <c r="D77" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>Contenções Paramento</v>
+      </c>
+      <c r="E77" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A78" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" s="20" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="79" spans="1:3">
-      <c r="A79" t="s">
+      <c r="D78" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>Contenções Grampo</v>
+      </c>
+      <c r="E78" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A79" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B79" s="20" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="80" spans="1:3">
-      <c r="A80" t="s">
+      <c r="D79" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>Contenções Dreno</v>
+      </c>
+      <c r="E79" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A80" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C80" s="20" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="81" spans="1:3">
-      <c r="A81" t="s">
+      <c r="D80" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>Pavimentação Camadas</v>
+      </c>
+      <c r="E80" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A81" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B81" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C81" s="20" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="82" spans="1:3">
-      <c r="A82" t="s">
+      <c r="D81" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>Pavimentação Camadas</v>
+      </c>
+      <c r="E81" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A82" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C82" s="20" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="83" spans="1:3">
-      <c r="A83" t="s">
+      <c r="D82" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>Pavimentação Camadas</v>
+      </c>
+      <c r="E82" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A83" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B83" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C83" s="20" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="84" spans="1:3">
-      <c r="A84" t="s">
+      <c r="D83" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>Pavimentação Camadas</v>
+      </c>
+      <c r="E83" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A84" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C84" s="20" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="85" spans="1:3">
-      <c r="A85" t="s">
+      <c r="D84" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>Pavimentação Camadas</v>
+      </c>
+      <c r="E84" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A85" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B85" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C85" s="20" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="86" spans="1:3">
-      <c r="A86" t="s">
+      <c r="D85" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>Pavimentação Camadas</v>
+      </c>
+      <c r="E85" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A86" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B86" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C86" s="20" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="87" spans="1:3">
-      <c r="A87" t="s">
+      <c r="D86" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>Pavimentação Camadas</v>
+      </c>
+      <c r="E86" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A87" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B87" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C87" s="20" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="88" spans="1:3">
-      <c r="A88" t="s">
+      <c r="D87" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>Pavimentação Camadas</v>
+      </c>
+      <c r="E87" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="24.95" customHeight="1">
+      <c r="A88" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B88" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C88" s="20" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="89" spans="1:3">
-      <c r="C89" t="s">
+      <c r="D88" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v>Pavimentação Camadas</v>
+      </c>
+      <c r="E88" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="24.95" customHeight="1">
+      <c r="C89" s="20" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="90" spans="1:3">
-      <c r="C90" t="s">
+      <c r="D89" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E89" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="24.95" customHeight="1">
+      <c r="C90" s="20" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="91" spans="1:3">
-      <c r="C91" t="s">
+      <c r="D90" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E90" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="24.95" customHeight="1">
+      <c r="C91" s="20" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="92" spans="1:3">
-      <c r="C92" t="s">
+      <c r="D91" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E91" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="24.95" customHeight="1">
+      <c r="C92" s="20" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="93" spans="1:3">
-      <c r="C93" t="s">
+      <c r="D92" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E92" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="24.95" customHeight="1">
+      <c r="C93" s="20" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="94" spans="1:3">
-      <c r="C94" t="s">
+      <c r="D93" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E93" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="24.95" customHeight="1">
+      <c r="C94" s="20" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="95" spans="1:3">
-      <c r="C95" t="s">
+      <c r="D94" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E94" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="24.95" customHeight="1">
+      <c r="C95" s="20" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="96" spans="1:3">
-      <c r="C96" t="s">
+      <c r="D95" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E95" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="24.95" customHeight="1">
+      <c r="C96" s="20" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="97" spans="3:4">
-      <c r="C97" t="s">
+      <c r="D96" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E96" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="97" spans="3:5" ht="24.95" customHeight="1">
+      <c r="C97" s="20" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="98" spans="3:4">
-      <c r="C98" t="s">
+      <c r="D97" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E97" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="98" spans="3:5" ht="24.95" customHeight="1">
+      <c r="C98" s="20" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="99" spans="3:4">
-      <c r="C99" t="s">
+      <c r="D98" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E98" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="99" spans="3:5" ht="24.95" customHeight="1">
+      <c r="C99" s="20" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="101" spans="3:4">
-      <c r="C101" t="s">
+      <c r="D99" s="20" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="E99" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="101" spans="3:5" ht="24.95" customHeight="1">
+      <c r="C101" s="20" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="102" spans="3:4">
-      <c r="C102" t="s">
+    <row r="102" spans="3:5" ht="24.95" customHeight="1">
+      <c r="C102" s="20" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="104" spans="3:4">
-      <c r="C104" t="s">
+    <row r="104" spans="3:5" ht="24.95" customHeight="1">
+      <c r="C104" s="20" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="105" spans="3:4">
-      <c r="C105" t="s">
+    <row r="105" spans="3:5" ht="24.95" customHeight="1">
+      <c r="C105" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="D105" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="106" spans="3:4">
-      <c r="C106" t="s">
+      <c r="D105" s="20" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="106" spans="3:5" ht="24.95" customHeight="1">
+      <c r="C106" s="20" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="107" spans="3:4">
-      <c r="C107" t="s">
+    <row r="107" spans="3:5" ht="24.95" customHeight="1">
+      <c r="C107" s="20" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="108" spans="3:4">
-      <c r="C108" t="s">
+    <row r="108" spans="3:5" ht="24.95" customHeight="1">
+      <c r="C108" s="20" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="109" spans="3:4">
-      <c r="C109" t="s">
+    <row r="109" spans="3:5" ht="24.95" customHeight="1">
+      <c r="C109" s="20" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="110" spans="3:4">
-      <c r="C110" t="s">
+    <row r="110" spans="3:5" ht="24.95" customHeight="1">
+      <c r="C110" s="20" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="111" spans="3:4">
-      <c r="C111" t="s">
+    <row r="111" spans="3:5" ht="24.95" customHeight="1">
+      <c r="C111" s="20" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="112" spans="3:4">
-      <c r="C112" t="s">
+    <row r="112" spans="3:5" ht="24.95" customHeight="1">
+      <c r="C112" s="20" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="113" spans="1:3">
-      <c r="C113" t="s">
+    <row r="113" spans="1:3" ht="24.95" customHeight="1">
+      <c r="C113" s="20" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="114" spans="1:3">
-      <c r="C114" t="s">
+    <row r="114" spans="1:3" ht="24.95" customHeight="1">
+      <c r="C114" s="20" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="115" spans="1:3">
-      <c r="C115" t="s">
+    <row r="115" spans="1:3" ht="24.95" customHeight="1">
+      <c r="C115" s="20" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="116" spans="1:3">
-      <c r="C116" t="s">
+    <row r="116" spans="1:3" ht="24.95" customHeight="1">
+      <c r="C116" s="20" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="117" spans="1:3">
-      <c r="C117" t="s">
+    <row r="117" spans="1:3" ht="24.95" customHeight="1">
+      <c r="C117" s="20" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="118" spans="1:3">
-      <c r="C118" t="s">
+    <row r="118" spans="1:3" ht="24.95" customHeight="1">
+      <c r="C118" s="20" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="119" spans="1:3">
-      <c r="C119" t="s">
+    <row r="119" spans="1:3" ht="24.95" customHeight="1">
+      <c r="C119" s="20" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="120" spans="1:3">
-      <c r="C120" t="s">
+    <row r="120" spans="1:3" ht="24.95" customHeight="1">
+      <c r="C120" s="20" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="121" spans="1:3">
-      <c r="C121" t="s">
+    <row r="121" spans="1:3" ht="24.95" customHeight="1">
+      <c r="C121" s="20" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="123" spans="1:3">
-      <c r="C123" t="s">
+    <row r="123" spans="1:3" ht="24.95" customHeight="1">
+      <c r="C123" s="20" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="124" spans="1:3">
-      <c r="C124" t="s">
+    <row r="124" spans="1:3" ht="24.95" customHeight="1">
+      <c r="C124" s="20" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="126" spans="1:3">
-      <c r="A126" t="s">
+    <row r="126" spans="1:3" ht="24.95" customHeight="1">
+      <c r="A126" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B126" s="20" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="128" spans="1:3">
-      <c r="A128" t="s">
+    <row r="128" spans="1:3" ht="24.95" customHeight="1">
+      <c r="A128" s="20" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="46c1aeda-4339-4b8b-a459-7d103ad23afd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7f741f0e-0184-4da7-b34a-985725fbfc5c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100420EFA20B37EED4A8F98A9C2EC890BB7" ma:contentTypeVersion="16" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="aea3d44a9351536121d93178e4f7fb0b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="46c1aeda-4339-4b8b-a459-7d103ad23afd" xmlns:ns3="7f741f0e-0184-4da7-b34a-985725fbfc5c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fa4f8d974e4007d34fcdac288d761fe2" ns2:_="" ns3:_="">
     <xsd:import namespace="46c1aeda-4339-4b8b-a459-7d103ad23afd"/>
@@ -2636,27 +3365,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD9B636E-1D90-4291-AF4B-712D7133623B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="7f741f0e-0184-4da7-b34a-985725fbfc5c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="46c1aeda-4339-4b8b-a459-7d103ad23afd"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="46c1aeda-4339-4b8b-a459-7d103ad23afd">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7f741f0e-0184-4da7-b34a-985725fbfc5c" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24BE5561-D38A-4410-949A-27D5851D1DDF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45B7DAC2-3615-4581-A9A5-5F14EE2CD8B7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2673,29 +3407,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24BE5561-D38A-4410-949A-27D5851D1DDF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD9B636E-1D90-4291-AF4B-712D7133623B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="7f741f0e-0184-4da7-b34a-985725fbfc5c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="46c1aeda-4339-4b8b-a459-7d103ad23afd"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>